<commit_message>
Added a development script to lay out the steps for getting lsmeans.
</commit_message>
<xml_diff>
--- a/data/yield/2021_USB 5 Early_PLY.xlsx
+++ b/data/yield/2021_USB 5 Early_PLY.xlsx
@@ -941,14 +941,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="13.140625" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>

</xml_diff>